<commit_message>
added 100 pin connector
</commit_message>
<xml_diff>
--- a/PCB(beta)/PartsToCADSpreadsheet.xlsx
+++ b/PCB(beta)/PartsToCADSpreadsheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Documents/Electrical Double Life/RoboJackets GitHub/roboracing-electrical/PCB(beta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\kendo\Google Drive\ECE\robojackets\Eagle\roboracing_desktop\roboracing-electrical\PCB(beta)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="25600" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="1440" yWindow="465" windowWidth="25605" windowHeight="15945" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -322,6 +322,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -651,24 +654,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="31.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -679,19 +682,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -702,7 +705,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -713,7 +716,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -722,7 +725,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -733,7 +736,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -744,7 +747,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -755,7 +758,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -766,7 +769,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -777,7 +780,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -788,7 +791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -799,7 +802,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -810,7 +813,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -821,7 +824,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -832,7 +835,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -843,30 +846,30 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -875,7 +878,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -886,7 +889,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -895,7 +898,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -906,7 +909,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -917,7 +920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -926,7 +929,7 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -937,7 +940,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -948,7 +951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>692122030100</v>
       </c>
@@ -959,7 +962,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -968,7 +971,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -979,7 +982,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
added usb power chip
</commit_message>
<xml_diff>
--- a/PCB(beta)/PartsToCADSpreadsheet.xlsx
+++ b/PCB(beta)/PartsToCADSpreadsheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>BK-916-TR</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>https://www.maximintegrated.com/en/products/analog/video-products/MAX9406.html</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/TPS2561DRCR/296-37670-1-ND/4833902</t>
+  </si>
+  <si>
+    <t>TPS2561DRCR</t>
   </si>
 </sst>
 </file>
@@ -655,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -863,145 +869,156 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>692122030100</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C32" r:id="rId1"/>
+    <hyperlink ref="C33" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>